<commit_message>
Pricesheet for Tue 09 Mar 2021 20:50:39 CAT
</commit_message>
<xml_diff>
--- a/xls-daily-price-sheets/09-03-2021.xlsx
+++ b/xls-daily-price-sheets/09-03-2021.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="184">
   <si>
     <t>Company Name</t>
   </si>
@@ -178,19 +178,19 @@
     <t>50.0000</t>
   </si>
   <si>
-    <t>2.1471</t>
+    <t>2.1843</t>
   </si>
   <si>
     <t>6.9704</t>
   </si>
   <si>
-    <t>2.2933</t>
-  </si>
-  <si>
-    <t>15.5793</t>
-  </si>
-  <si>
-    <t>6.4856</t>
+    <t>2.1517</t>
+  </si>
+  <si>
+    <t>15.9466</t>
+  </si>
+  <si>
+    <t>6.5045</t>
   </si>
   <si>
     <t>870.0000</t>
@@ -199,241 +199,250 @@
     <t>110.6667</t>
   </si>
   <si>
-    <t>14.9572</t>
-  </si>
-  <si>
-    <t>96.3562</t>
-  </si>
-  <si>
-    <t>17.9818</t>
-  </si>
-  <si>
-    <t>49.9476</t>
-  </si>
-  <si>
-    <t>20.2227</t>
-  </si>
-  <si>
-    <t>3.9933</t>
-  </si>
-  <si>
-    <t>28.0095</t>
-  </si>
-  <si>
-    <t>5.0000</t>
-  </si>
-  <si>
-    <t>1.5378</t>
-  </si>
-  <si>
-    <t>21.1902</t>
-  </si>
-  <si>
-    <t>5.4500</t>
-  </si>
-  <si>
-    <t>0.5874</t>
+    <t>14.9563</t>
+  </si>
+  <si>
+    <t>97.0000</t>
+  </si>
+  <si>
+    <t>19.4000</t>
+  </si>
+  <si>
+    <t>49.1609</t>
+  </si>
+  <si>
+    <t>20.2035</t>
+  </si>
+  <si>
+    <t>4.0000</t>
+  </si>
+  <si>
+    <t>30.0000</t>
+  </si>
+  <si>
+    <t>5.1000</t>
+  </si>
+  <si>
+    <t>1.5145</t>
+  </si>
+  <si>
+    <t>21.0000</t>
+  </si>
+  <si>
+    <t>5.4906</t>
+  </si>
+  <si>
+    <t>0.6179</t>
   </si>
   <si>
     <t>0.3500</t>
   </si>
   <si>
-    <t>130.2000</t>
-  </si>
-  <si>
-    <t>63.4876</t>
+    <t>115.1892</t>
+  </si>
+  <si>
+    <t>63.5000</t>
   </si>
   <si>
     <t>39.6000</t>
   </si>
   <si>
-    <t>1.8033</t>
+    <t>1.7485</t>
   </si>
   <si>
     <t>17.0000</t>
   </si>
   <si>
-    <t>0.0700</t>
-  </si>
-  <si>
-    <t>45.9750</t>
-  </si>
-  <si>
-    <t>9.8900</t>
-  </si>
-  <si>
-    <t>319.3000</t>
-  </si>
-  <si>
-    <t>2.4225</t>
+    <t>0.0709</t>
+  </si>
+  <si>
+    <t>49.5003</t>
+  </si>
+  <si>
+    <t>9.8088</t>
+  </si>
+  <si>
+    <t>319.0391</t>
+  </si>
+  <si>
+    <t>2.9050</t>
   </si>
   <si>
     <t>7.4800</t>
   </si>
   <si>
-    <t>15.0418</t>
-  </si>
-  <si>
-    <t>40.4574</t>
+    <t>15.7287</t>
+  </si>
+  <si>
+    <t>40.2559</t>
   </si>
   <si>
     <t>22.9922</t>
   </si>
   <si>
-    <t>1.9991</t>
-  </si>
-  <si>
-    <t>21.0000</t>
+    <t>1.9000</t>
+  </si>
+  <si>
+    <t>21.0500</t>
   </si>
   <si>
     <t>21.6089</t>
   </si>
   <si>
-    <t>25.0036</t>
-  </si>
-  <si>
-    <t>0.4999</t>
-  </si>
-  <si>
-    <t>0.8339</t>
+    <t>25.3810</t>
+  </si>
+  <si>
+    <t>0.4735</t>
+  </si>
+  <si>
+    <t>0.8309</t>
+  </si>
+  <si>
+    <t>44.9500</t>
+  </si>
+  <si>
+    <t>3.1075</t>
+  </si>
+  <si>
+    <t>11.1308</t>
+  </si>
+  <si>
+    <t>0.8103</t>
+  </si>
+  <si>
+    <t>39.7500</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>1.3400</t>
+  </si>
+  <si>
+    <t>8.2385</t>
+  </si>
+  <si>
+    <t>1.9594</t>
+  </si>
+  <si>
+    <t>Closing Price</t>
+  </si>
+  <si>
+    <t>2.5005</t>
+  </si>
+  <si>
+    <t>6.9763</t>
+  </si>
+  <si>
+    <t>2.1444</t>
+  </si>
+  <si>
+    <t>16.0000</t>
+  </si>
+  <si>
+    <t>6.5077</t>
+  </si>
+  <si>
+    <t>113.7500</t>
+  </si>
+  <si>
+    <t>14.9395</t>
+  </si>
+  <si>
+    <t>84.4805</t>
+  </si>
+  <si>
+    <t>18.2934</t>
+  </si>
+  <si>
+    <t>49.0763</t>
+  </si>
+  <si>
+    <t>20.0139</t>
+  </si>
+  <si>
+    <t>4.0190</t>
+  </si>
+  <si>
+    <t>28.0149</t>
+  </si>
+  <si>
+    <t>5.9419</t>
+  </si>
+  <si>
+    <t>1.7024</t>
+  </si>
+  <si>
+    <t>5.4400</t>
+  </si>
+  <si>
+    <t>0.6530</t>
+  </si>
+  <si>
+    <t>118.4900</t>
+  </si>
+  <si>
+    <t>63.9878</t>
+  </si>
+  <si>
+    <t>40.0000</t>
+  </si>
+  <si>
+    <t>1.9764</t>
+  </si>
+  <si>
+    <t>18.0000</t>
+  </si>
+  <si>
+    <t>0.0835</t>
+  </si>
+  <si>
+    <t>49.6600</t>
+  </si>
+  <si>
+    <t>9.6923</t>
+  </si>
+  <si>
+    <t>7.4567</t>
+  </si>
+  <si>
+    <t>16.0276</t>
+  </si>
+  <si>
+    <t>39.5815</t>
+  </si>
+  <si>
+    <t>22.7171</t>
+  </si>
+  <si>
+    <t>2.0379</t>
+  </si>
+  <si>
+    <t>29.9890</t>
+  </si>
+  <si>
+    <t>0.4723</t>
+  </si>
+  <si>
+    <t>0.8465</t>
   </si>
   <si>
     <t>43.0000</t>
   </si>
   <si>
-    <t>2.5900</t>
-  </si>
-  <si>
-    <t>9.9974</t>
-  </si>
-  <si>
-    <t>0.7627</t>
-  </si>
-  <si>
-    <t>39.7500</t>
-  </si>
-  <si>
-    <t>0.0002</t>
-  </si>
-  <si>
-    <t>1.3400</t>
-  </si>
-  <si>
-    <t>7.7993</t>
-  </si>
-  <si>
-    <t>1.9474</t>
-  </si>
-  <si>
-    <t>Closing Price</t>
-  </si>
-  <si>
-    <t>2.1843</t>
-  </si>
-  <si>
-    <t>2.1517</t>
-  </si>
-  <si>
-    <t>15.9466</t>
-  </si>
-  <si>
-    <t>6.5045</t>
-  </si>
-  <si>
-    <t>14.9563</t>
-  </si>
-  <si>
-    <t>97.0000</t>
-  </si>
-  <si>
-    <t>19.4000</t>
-  </si>
-  <si>
-    <t>49.1609</t>
-  </si>
-  <si>
-    <t>20.2035</t>
-  </si>
-  <si>
-    <t>4.0000</t>
-  </si>
-  <si>
-    <t>30.0000</t>
-  </si>
-  <si>
-    <t>5.1000</t>
-  </si>
-  <si>
-    <t>1.5145</t>
-  </si>
-  <si>
-    <t>5.4906</t>
-  </si>
-  <si>
-    <t>0.6179</t>
-  </si>
-  <si>
-    <t>115.1892</t>
-  </si>
-  <si>
-    <t>63.5000</t>
-  </si>
-  <si>
-    <t>1.7485</t>
-  </si>
-  <si>
-    <t>0.0709</t>
-  </si>
-  <si>
-    <t>49.5003</t>
-  </si>
-  <si>
-    <t>9.8088</t>
-  </si>
-  <si>
-    <t>319.0391</t>
-  </si>
-  <si>
-    <t>2.9050</t>
-  </si>
-  <si>
-    <t>15.7287</t>
-  </si>
-  <si>
-    <t>40.2559</t>
-  </si>
-  <si>
-    <t>1.9000</t>
-  </si>
-  <si>
-    <t>21.0500</t>
-  </si>
-  <si>
-    <t>25.3810</t>
-  </si>
-  <si>
-    <t>0.4735</t>
-  </si>
-  <si>
-    <t>0.8309</t>
-  </si>
-  <si>
-    <t>44.9500</t>
-  </si>
-  <si>
-    <t>3.1075</t>
-  </si>
-  <si>
-    <t>11.1308</t>
-  </si>
-  <si>
-    <t>0.8103</t>
-  </si>
-  <si>
-    <t>8.2385</t>
-  </si>
-  <si>
-    <t>1.9594</t>
+    <t>3.5010</t>
+  </si>
+  <si>
+    <t>11.0648</t>
+  </si>
+  <si>
+    <t>0.8556</t>
+  </si>
+  <si>
+    <t>7.9778</t>
+  </si>
+  <si>
+    <t>1.9539</t>
   </si>
   <si>
     <t>Total Traded Volume</t>
@@ -442,115 +451,121 @@
     <t>0</t>
   </si>
   <si>
-    <t>5400</t>
-  </si>
-  <si>
-    <t>4653000</t>
-  </si>
-  <si>
-    <t>84700</t>
-  </si>
-  <si>
-    <t>258400</t>
-  </si>
-  <si>
-    <t>69600</t>
-  </si>
-  <si>
-    <t>1500</t>
+    <t>149000</t>
+  </si>
+  <si>
+    <t>16700</t>
+  </si>
+  <si>
+    <t>6200</t>
+  </si>
+  <si>
+    <t>579500</t>
+  </si>
+  <si>
+    <t>24400</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>454700</t>
+  </si>
+  <si>
+    <t>8276729</t>
+  </si>
+  <si>
+    <t>6100</t>
+  </si>
+  <si>
+    <t>563800</t>
+  </si>
+  <si>
+    <t>1700600</t>
+  </si>
+  <si>
+    <t>12600</t>
+  </si>
+  <si>
+    <t>26900</t>
+  </si>
+  <si>
+    <t>3100</t>
+  </si>
+  <si>
+    <t>39800</t>
+  </si>
+  <si>
+    <t>2400</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>15500</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>129600</t>
+  </si>
+  <si>
+    <t>21500</t>
+  </si>
+  <si>
+    <t>426200</t>
+  </si>
+  <si>
+    <t>146600</t>
+  </si>
+  <si>
+    <t>1300</t>
   </si>
   <si>
     <t>900</t>
   </si>
   <si>
-    <t>387700</t>
-  </si>
-  <si>
-    <t>37000</t>
-  </si>
-  <si>
-    <t>27900</t>
-  </si>
-  <si>
-    <t>200</t>
+    <t>632800</t>
+  </si>
+  <si>
+    <t>11100</t>
+  </si>
+  <si>
+    <t>14300</t>
+  </si>
+  <si>
+    <t>161000</t>
+  </si>
+  <si>
+    <t>7000</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>157400</t>
+  </si>
+  <si>
+    <t>80100</t>
+  </si>
+  <si>
+    <t>20800</t>
+  </si>
+  <si>
+    <t>27000</t>
+  </si>
+  <si>
+    <t>419100</t>
   </si>
   <si>
     <t>500</t>
   </si>
   <si>
-    <t>1802900</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>1600</t>
-  </si>
-  <si>
-    <t>8900</t>
-  </si>
-  <si>
-    <t>7400</t>
-  </si>
-  <si>
-    <t>65900</t>
-  </si>
-  <si>
-    <t>13400</t>
-  </si>
-  <si>
-    <t>17100</t>
-  </si>
-  <si>
-    <t>12973900</t>
-  </si>
-  <si>
-    <t>185800</t>
-  </si>
-  <si>
-    <t>3300</t>
-  </si>
-  <si>
-    <t>2300</t>
-  </si>
-  <si>
-    <t>7500</t>
-  </si>
-  <si>
-    <t>2800</t>
-  </si>
-  <si>
-    <t>314700</t>
-  </si>
-  <si>
-    <t>25600</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>8400</t>
-  </si>
-  <si>
-    <t>240700</t>
-  </si>
-  <si>
-    <t>35900</t>
-  </si>
-  <si>
-    <t>15600</t>
-  </si>
-  <si>
-    <t>34200</t>
-  </si>
-  <si>
-    <t>1300</t>
-  </si>
-  <si>
-    <t>2600</t>
-  </si>
-  <si>
-    <t>974700</t>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>313600</t>
   </si>
 </sst>
 </file>
@@ -939,7 +954,7 @@
         <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -958,7 +973,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -972,7 +987,7 @@
         <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -983,10 +998,10 @@
         <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -997,10 +1012,10 @@
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1011,10 +1026,10 @@
         <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1025,10 +1040,10 @@
         <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1042,7 +1057,7 @@
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1053,10 +1068,10 @@
         <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1067,10 +1082,10 @@
         <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1081,10 +1096,10 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1095,10 +1110,10 @@
         <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1109,10 +1124,10 @@
         <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1123,10 +1138,10 @@
         <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1137,10 +1152,10 @@
         <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1151,10 +1166,10 @@
         <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1165,10 +1180,10 @@
         <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1179,10 +1194,10 @@
         <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1193,10 +1208,10 @@
         <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1207,10 +1222,10 @@
         <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1221,10 +1236,10 @@
         <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1238,7 +1253,7 @@
         <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1249,10 +1264,10 @@
         <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1263,10 +1278,10 @@
         <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1277,10 +1292,10 @@
         <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1291,10 +1306,10 @@
         <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1305,10 +1320,10 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1319,10 +1334,10 @@
         <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1333,10 +1348,10 @@
         <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1347,10 +1362,10 @@
         <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D36" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1361,10 +1376,10 @@
         <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1375,10 +1390,10 @@
         <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1389,10 +1404,10 @@
         <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1403,10 +1418,10 @@
         <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1417,10 +1432,10 @@
         <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1431,10 +1446,10 @@
         <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1445,10 +1460,10 @@
         <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1459,10 +1474,10 @@
         <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1476,7 +1491,7 @@
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1487,10 +1502,10 @@
         <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1501,10 +1516,10 @@
         <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1515,10 +1530,10 @@
         <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D48" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1529,10 +1544,10 @@
         <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1543,10 +1558,10 @@
         <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1557,10 +1572,10 @@
         <v>96</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1571,10 +1586,10 @@
         <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1588,7 +1603,7 @@
         <v>98</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1602,7 +1617,7 @@
         <v>99</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1616,7 +1631,7 @@
         <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1627,10 +1642,10 @@
         <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D56" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1641,10 +1656,10 @@
         <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>